<commit_message>
Added the case for reading blank cells as empty strings in place of 'NULL' strings.
</commit_message>
<xml_diff>
--- a/core-plugins/src/test/resources/civil_test_data_two.xlsx
+++ b/core-plugins/src/test/resources/civil_test_data_two.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Alan</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>designer</t>
+  </si>
+  <si>
+    <t>Ruskin</t>
   </si>
   <si>
     <t>writer</t>
@@ -59,12 +62,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
@@ -86,12 +93,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -354,6 +364,9 @@
       <c r="A3" s="1">
         <v>10</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="1">
         <v>56</v>
       </c>
@@ -361,7 +374,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2">
         <v>43101</v>
@@ -372,16 +385,16 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2">
         <v>43101</v>
@@ -392,7 +405,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>46</v>
@@ -401,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2">
         <v>43101</v>
@@ -412,16 +425,16 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2">
         <v>43101</v>

</xml_diff>